<commit_message>
Structuring, bug fixes and IP support for SVI intf
IP complaincy for SVI interfaces.  Cut large code block in several functions. Bug fixes in interface complaincy reports.
</commit_message>
<xml_diff>
--- a/TestSwitch.xlsx
+++ b/TestSwitch.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>The following VLANs are present on the switch: 10,11,12,13</t>
   </si>
@@ -38,6 +38,9 @@
     <t>carrier-delay</t>
   </si>
   <si>
+    <t>cdp enable</t>
+  </si>
+  <si>
     <t>channel-group</t>
   </si>
   <si>
@@ -170,6 +173,9 @@
     <t>GigabitEthernet1/0/23</t>
   </si>
   <si>
+    <t xml:space="preserve"> no cdp enable</t>
+  </si>
+  <si>
     <t>GigabitEthernet1/0/24</t>
   </si>
   <si>
@@ -221,13 +227,31 @@
     <t>name</t>
   </si>
   <si>
+    <t>ip access-group</t>
+  </si>
+  <si>
+    <t>ip proxy arp</t>
+  </si>
+  <si>
+    <t>ip redirects</t>
+  </si>
+  <si>
     <t>Ten</t>
   </si>
   <si>
     <t>1.2.3.4 255.255.255.0</t>
   </si>
   <si>
+    <t xml:space="preserve"> no ip proxy arp</t>
+  </si>
+  <si>
     <t>Eleven</t>
+  </si>
+  <si>
+    <t>10 in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no ip redirects</t>
   </si>
   <si>
     <t>Twelfe</t>
@@ -609,7 +633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,22 +646,23 @@
     <col customWidth="1" max="3" min="3" width="15"/>
     <col customWidth="1" max="4" min="4" width="16"/>
     <col customWidth="1" max="5" min="5" width="16"/>
-    <col customWidth="1" max="6" min="6" width="20"/>
-    <col customWidth="1" max="7" min="7" width="13"/>
-    <col customWidth="1" max="8" min="8" width="37"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="15"/>
-    <col customWidth="1" max="11" min="11" width="26"/>
-    <col customWidth="1" max="12" min="12" width="24"/>
-    <col customWidth="1" max="13" min="13" width="22"/>
-    <col customWidth="1" max="14" min="14" width="31"/>
-    <col customWidth="1" max="15" min="15" width="13"/>
-    <col customWidth="1" max="16" min="16" width="24"/>
-    <col customWidth="1" max="17" min="17" width="17"/>
-    <col customWidth="1" max="18" min="18" width="16"/>
+    <col customWidth="1" max="6" min="6" width="16"/>
+    <col customWidth="1" max="7" min="7" width="20"/>
+    <col customWidth="1" max="8" min="8" width="13"/>
+    <col customWidth="1" max="9" min="9" width="37"/>
+    <col customWidth="1" max="10" min="10" width="10"/>
+    <col customWidth="1" max="11" min="11" width="15"/>
+    <col customWidth="1" max="12" min="12" width="26"/>
+    <col customWidth="1" max="13" min="13" width="24"/>
+    <col customWidth="1" max="14" min="14" width="22"/>
+    <col customWidth="1" max="15" min="15" width="31"/>
+    <col customWidth="1" max="16" min="16" width="13"/>
+    <col customWidth="1" max="17" min="17" width="24"/>
+    <col customWidth="1" max="18" min="18" width="17"/>
+    <col customWidth="1" max="19" min="19" width="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -692,13 +717,16 @@
       <c r="R1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s"/>
       <c r="D2" t="s"/>
@@ -709,135 +737,139 @@
       <c r="I2" t="s"/>
       <c r="J2" t="s"/>
       <c r="K2" t="s"/>
-      <c r="L2" t="s">
+      <c r="L2" t="s"/>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s"/>
+      <c r="O2" t="s"/>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s"/>
+      <c r="R2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" t="s"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" t="s"/>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3" t="s"/>
       <c r="D3" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
       <c r="G3" t="s"/>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s"/>
-      <c r="J3" t="s">
+      <c r="H3" t="s"/>
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s"/>
+      <c r="J3" t="s"/>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
       <c r="L3" t="s"/>
       <c r="M3" t="s"/>
       <c r="N3" t="s"/>
       <c r="O3" t="s"/>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
+      <c r="P3" t="s"/>
       <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" t="s"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s"/>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="s"/>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s"/>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" t="s"/>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" t="s"/>
+      <c r="K4" t="s"/>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
       <c r="M4" t="s"/>
       <c r="N4" t="s"/>
       <c r="O4" t="s"/>
-      <c r="P4" t="s">
-        <v>32</v>
-      </c>
+      <c r="P4" t="s"/>
       <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s"/>
-    </row>
-    <row r="5" spans="1:18">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" t="s"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s"/>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
       <c r="G5" t="s"/>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s"/>
-      <c r="J5" t="s">
+      <c r="H5" t="s"/>
+      <c r="I5" t="s">
         <v>27</v>
       </c>
-      <c r="K5" t="s"/>
+      <c r="J5" t="s"/>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
       <c r="L5" t="s"/>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
+      <c r="M5" t="s"/>
       <c r="N5" t="s">
         <v>35</v>
       </c>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s">
+      <c r="O5" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" t="s"/>
+      <c r="P5" t="s"/>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
       <c r="R5" t="s"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" t="s"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s"/>
       <c r="C6" t="s"/>
       <c r="D6" t="s"/>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
+      <c r="E6" t="s"/>
       <c r="F6" t="s">
         <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" t="s"/>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
       <c r="I6" t="s"/>
       <c r="J6" t="s"/>
       <c r="K6" t="s"/>
@@ -847,22 +879,23 @@
       <c r="O6" t="s"/>
       <c r="P6" t="s"/>
       <c r="Q6" t="s"/>
-      <c r="R6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" t="s"/>
+      <c r="S6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s"/>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s"/>
+      <c r="D7" t="s"/>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
       <c r="F7" t="s"/>
       <c r="G7" t="s"/>
       <c r="H7" t="s"/>
@@ -870,33 +903,34 @@
       <c r="J7" t="s"/>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
-      <c r="M7" t="s">
-        <v>34</v>
-      </c>
+      <c r="M7" t="s"/>
       <c r="N7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" t="s"/>
-      <c r="P7" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7" t="s"/>
       <c r="Q7" t="s">
         <v>29</v>
       </c>
-      <c r="R7" t="s"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" t="s"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s"/>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s"/>
+      <c r="D8" t="s"/>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
       <c r="F8" t="s"/>
       <c r="G8" t="s"/>
       <c r="H8" t="s"/>
@@ -904,33 +938,34 @@
       <c r="J8" t="s"/>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
+      <c r="M8" t="s"/>
       <c r="N8" t="s">
-        <v>44</v>
-      </c>
-      <c r="O8" t="s"/>
-      <c r="P8" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" t="s"/>
       <c r="Q8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" t="s"/>
-    </row>
-    <row r="9" spans="1:18">
+        <v>33</v>
+      </c>
+      <c r="R8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" t="s"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s"/>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s"/>
+      <c r="D9" t="s"/>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" t="s"/>
       <c r="G9" t="s"/>
       <c r="H9" t="s"/>
@@ -939,56 +974,62 @@
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" t="s"/>
-      <c r="P9" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="O9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" t="s"/>
       <c r="Q9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" t="s"/>
-    </row>
-    <row r="10" spans="1:18">
+        <v>37</v>
+      </c>
+      <c r="R9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" t="s"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s"/>
-      <c r="D10" t="s"/>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
       <c r="G10" t="s"/>
       <c r="H10" t="s"/>
       <c r="I10" t="s"/>
       <c r="J10" t="s"/>
-      <c r="K10" t="s">
-        <v>31</v>
-      </c>
+      <c r="K10" t="s"/>
       <c r="L10" t="s"/>
       <c r="M10" t="s"/>
       <c r="N10" t="s"/>
       <c r="O10" t="s"/>
       <c r="P10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q10" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" t="s"/>
-    </row>
-    <row r="11" spans="1:18">
+        <v>33</v>
+      </c>
+      <c r="R10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" t="s"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s"/>
       <c r="D11" t="s"/>
@@ -997,25 +1038,26 @@
       <c r="G11" t="s"/>
       <c r="H11" t="s"/>
       <c r="I11" t="s"/>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s"/>
+      <c r="J11" t="s"/>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
       <c r="L11" t="s"/>
       <c r="M11" t="s"/>
       <c r="N11" t="s"/>
       <c r="O11" t="s"/>
-      <c r="P11" t="s">
-        <v>36</v>
-      </c>
+      <c r="P11" t="s"/>
       <c r="Q11" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" t="s"/>
-    </row>
-    <row r="12" spans="1:18">
+        <v>37</v>
+      </c>
+      <c r="R11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" t="s"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s"/>
       <c r="C12" t="s"/>
@@ -1034,10 +1076,11 @@
       <c r="P12" t="s"/>
       <c r="Q12" t="s"/>
       <c r="R12" t="s"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="S12" t="s"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s"/>
       <c r="C13" t="s"/>
@@ -1046,10 +1089,10 @@
       <c r="F13" t="s"/>
       <c r="G13" t="s"/>
       <c r="H13" t="s"/>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s"/>
+      <c r="I13" t="s"/>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
       <c r="M13" t="s"/>
@@ -1058,10 +1101,11 @@
       <c r="P13" t="s"/>
       <c r="Q13" t="s"/>
       <c r="R13" t="s"/>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" t="s"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s"/>
       <c r="C14" t="s"/>
@@ -1070,10 +1114,10 @@
       <c r="F14" t="s"/>
       <c r="G14" t="s"/>
       <c r="H14" t="s"/>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s"/>
+      <c r="I14" t="s"/>
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
       <c r="K14" t="s"/>
       <c r="L14" t="s"/>
       <c r="M14" t="s"/>
@@ -1082,10 +1126,11 @@
       <c r="P14" t="s"/>
       <c r="Q14" t="s"/>
       <c r="R14" t="s"/>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" t="s"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s"/>
       <c r="C15" t="s"/>
@@ -1104,19 +1149,20 @@
       <c r="P15" t="s"/>
       <c r="Q15" t="s"/>
       <c r="R15" t="s"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" t="s"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s"/>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s"/>
+      <c r="D16" t="s"/>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
       <c r="F16" t="s"/>
       <c r="G16" t="s"/>
       <c r="H16" t="s"/>
@@ -1126,18 +1172,19 @@
       <c r="L16" t="s"/>
       <c r="M16" t="s"/>
       <c r="N16" t="s"/>
-      <c r="O16" t="s">
+      <c r="O16" t="s"/>
+      <c r="P16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16" t="s"/>
+      <c r="R16" t="s">
         <v>24</v>
       </c>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s">
-        <v>23</v>
-      </c>
-      <c r="R16" t="s"/>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" t="s"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s"/>
       <c r="C17" t="s"/>
@@ -1146,10 +1193,10 @@
       <c r="F17" t="s"/>
       <c r="G17" t="s"/>
       <c r="H17" t="s"/>
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s"/>
+      <c r="I17" t="s"/>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
       <c r="K17" t="s"/>
       <c r="L17" t="s"/>
       <c r="M17" t="s"/>
@@ -1158,10 +1205,11 @@
       <c r="P17" t="s"/>
       <c r="Q17" t="s"/>
       <c r="R17" t="s"/>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" t="s"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s"/>
       <c r="C18" t="s"/>
@@ -1170,10 +1218,10 @@
       <c r="F18" t="s"/>
       <c r="G18" t="s"/>
       <c r="H18" t="s"/>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s"/>
+      <c r="I18" t="s"/>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
       <c r="K18" t="s"/>
       <c r="L18" t="s"/>
       <c r="M18" t="s"/>
@@ -1182,10 +1230,11 @@
       <c r="P18" t="s"/>
       <c r="Q18" t="s"/>
       <c r="R18" t="s"/>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" t="s"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s"/>
       <c r="C19" t="s"/>
@@ -1194,10 +1243,10 @@
       <c r="F19" t="s"/>
       <c r="G19" t="s"/>
       <c r="H19" t="s"/>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" t="s"/>
+      <c r="I19" t="s"/>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
       <c r="K19" t="s"/>
       <c r="L19" t="s"/>
       <c r="M19" t="s"/>
@@ -1206,19 +1255,20 @@
       <c r="P19" t="s"/>
       <c r="Q19" t="s"/>
       <c r="R19" t="s"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" t="s"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s"/>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="s"/>
+      <c r="D20" t="s"/>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
       <c r="F20" t="s"/>
       <c r="G20" t="s"/>
       <c r="H20" t="s"/>
@@ -1226,33 +1276,34 @@
       <c r="J20" t="s"/>
       <c r="K20" t="s"/>
       <c r="L20" t="s"/>
-      <c r="M20" t="s">
-        <v>34</v>
-      </c>
+      <c r="M20" t="s"/>
       <c r="N20" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20" t="s"/>
-      <c r="P20" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
+      <c r="P20" t="s"/>
       <c r="Q20" t="s">
         <v>29</v>
       </c>
-      <c r="R20" t="s"/>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="R20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" t="s"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s"/>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s"/>
+      <c r="D21" t="s"/>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
       <c r="F21" t="s"/>
       <c r="G21" t="s"/>
       <c r="H21" t="s"/>
@@ -1263,26 +1314,27 @@
       <c r="M21" t="s"/>
       <c r="N21" t="s"/>
       <c r="O21" t="s"/>
-      <c r="P21" t="s">
-        <v>32</v>
-      </c>
+      <c r="P21" t="s"/>
       <c r="Q21" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21" t="s"/>
-    </row>
-    <row r="22" spans="1:18">
+        <v>33</v>
+      </c>
+      <c r="R21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" t="s"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s"/>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" t="s"/>
+      <c r="D22" t="s"/>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
       <c r="F22" t="s"/>
       <c r="G22" t="s"/>
       <c r="H22" t="s"/>
@@ -1293,28 +1345,29 @@
       <c r="M22" t="s"/>
       <c r="N22" t="s"/>
       <c r="O22" t="s"/>
-      <c r="P22" t="s">
-        <v>36</v>
-      </c>
+      <c r="P22" t="s"/>
       <c r="Q22" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22" t="s"/>
-    </row>
-    <row r="23" spans="1:18">
+        <v>37</v>
+      </c>
+      <c r="R22" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" t="s"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" t="s"/>
+        <v>66</v>
+      </c>
+      <c r="D23" t="s"/>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
       <c r="F23" t="s"/>
       <c r="G23" t="s"/>
       <c r="H23" t="s"/>
@@ -1324,14 +1377,15 @@
       <c r="L23" t="s"/>
       <c r="M23" t="s"/>
       <c r="N23" t="s"/>
-      <c r="O23" t="s">
+      <c r="O23" t="s"/>
+      <c r="P23" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q23" t="s"/>
+      <c r="R23" t="s">
         <v>24</v>
       </c>
-      <c r="P23" t="s"/>
-      <c r="Q23" t="s">
-        <v>23</v>
-      </c>
-      <c r="R23" t="s"/>
+      <c r="S23" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1344,7 +1398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1354,67 +1408,99 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="6"/>
     <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="23"/>
-    <col customWidth="1" max="4" min="4" width="20"/>
+    <col customWidth="1" max="3" min="3" width="17"/>
+    <col customWidth="1" max="4" min="4" width="23"/>
+    <col customWidth="1" max="5" min="5" width="18"/>
+    <col customWidth="1" max="6" min="6" width="18"/>
+    <col customWidth="1" max="7" min="7" width="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C2" t="s"/>
       <c r="D2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s"/>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s"/>
-      <c r="D3" t="s"/>
-    </row>
-    <row r="4" spans="1:4">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s"/>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s"/>
       <c r="D4" t="s"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s"/>
+      <c r="F4" t="s"/>
+      <c r="G4" t="s"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s"/>
       <c r="D5" t="s"/>
+      <c r="E5" t="s"/>
+      <c r="F5" t="s"/>
+      <c r="G5" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>